<commit_message>
Fluxograma e ideia base do projeto em ppt
</commit_message>
<xml_diff>
--- a/Introdu-o-e-desenvolvimento-da-linguagem-de-programa-o-Java---grupo-1.xlsx
+++ b/Introdu-o-e-desenvolvimento-da-linguagem-de-programa-o-Java---grupo-1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A4B5A8-D3DF-4B07-9CAC-23CC29EEADC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA991367-3A76-41F8-91F2-F792B8EDC308}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="15040" windowHeight="10340" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapa Mental" sheetId="8" r:id="rId1"/>
@@ -303,6 +303,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -311,12 +327,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,6 +340,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,22 +354,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -435,16 +435,6 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Funcionaria</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -452,18 +442,8 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t> como um software link dentro de outros apps para que a mulhres pudesse denunciar</a:t>
+            <a:t>como um software link dentro de outros apps para que a mulhres pudesse denunciar</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2229,7 +2209,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>226089</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>38957</xdr:rowOff>
+      <xdr:rowOff>162278</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2246,8 +2226,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1956688" y="3948086"/>
-          <a:ext cx="2067714" cy="754031"/>
+          <a:off x="1962142" y="3903458"/>
+          <a:ext cx="2073947" cy="866098"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -2302,7 +2282,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> "Você será direcionado para um atendente" (envia para o centro de ajuda online</a:t>
+            <a:t> "Você será direcionado para um atendente" (envia para o centro de ajuda online)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -2440,13 +2420,13 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>226089</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>54199</xdr:rowOff>
+      <xdr:rowOff>55605</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>238789</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>20347</xdr:rowOff>
+      <xdr:rowOff>82007</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2464,8 +2444,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4024402" y="3462941"/>
-          <a:ext cx="12700" cy="862161"/>
+          <a:off x="4036089" y="3428161"/>
+          <a:ext cx="12700" cy="908346"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -3035,13 +3015,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>171410</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>20348</xdr:rowOff>
+      <xdr:rowOff>82008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>184141</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>135381</xdr:rowOff>
+      <xdr:rowOff>133975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3060,8 +3040,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1">
-          <a:off x="1943956" y="4325103"/>
-          <a:ext cx="12731" cy="1011045"/>
+          <a:off x="1949410" y="4336508"/>
+          <a:ext cx="12731" cy="933911"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -8223,7 +8203,7 @@
   </sheetPr>
   <dimension ref="B1:AW28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -8236,111 +8216,111 @@
   <sheetData>
     <row r="1" spans="2:49" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:49" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="11"/>
-      <c r="AQ2" s="11"/>
-      <c r="AR2" s="11"/>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="11"/>
-      <c r="AU2" s="11"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="13"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="13"/>
+      <c r="AP2" s="13"/>
+      <c r="AQ2" s="13"/>
+      <c r="AR2" s="13"/>
+      <c r="AS2" s="13"/>
+      <c r="AT2" s="13"/>
+      <c r="AU2" s="13"/>
     </row>
     <row r="3" spans="2:49" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
-      <c r="AH3" s="20"/>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="20"/>
-      <c r="AK3" s="20"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
       <c r="AL3" s="4"/>
     </row>
     <row r="4" spans="2:49" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="AK12" s="13" t="s">
+      <c r="AK12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="AL12" s="14"/>
-      <c r="AM12" s="14"/>
-      <c r="AN12" s="14"/>
-      <c r="AO12" s="14"/>
-      <c r="AP12" s="14"/>
-      <c r="AQ12" s="14"/>
-      <c r="AR12" s="14"/>
-      <c r="AS12" s="14"/>
-      <c r="AT12" s="14"/>
-      <c r="AU12" s="15"/>
+      <c r="AL12" s="18"/>
+      <c r="AM12" s="18"/>
+      <c r="AN12" s="18"/>
+      <c r="AO12" s="18"/>
+      <c r="AP12" s="18"/>
+      <c r="AQ12" s="18"/>
+      <c r="AR12" s="18"/>
+      <c r="AS12" s="18"/>
+      <c r="AT12" s="18"/>
+      <c r="AU12" s="19"/>
     </row>
     <row r="13" spans="2:49" x14ac:dyDescent="0.3">
       <c r="AK13" s="5" t="s">
@@ -8360,56 +8340,56 @@
       <c r="AW13" s="7"/>
     </row>
     <row r="14" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="9"/>
-      <c r="AM14" s="9"/>
-      <c r="AN14" s="9"/>
-      <c r="AO14" s="9"/>
-      <c r="AP14" s="9"/>
-      <c r="AQ14" s="9"/>
-      <c r="AR14" s="9"/>
-      <c r="AS14" s="9"/>
-      <c r="AT14" s="9"/>
-      <c r="AU14" s="10"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+      <c r="AN14" s="15"/>
+      <c r="AO14" s="15"/>
+      <c r="AP14" s="15"/>
+      <c r="AQ14" s="15"/>
+      <c r="AR14" s="15"/>
+      <c r="AS14" s="15"/>
+      <c r="AT14" s="15"/>
+      <c r="AU14" s="16"/>
     </row>
     <row r="15" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="AK15" s="8"/>
-      <c r="AL15" s="9"/>
-      <c r="AM15" s="9"/>
-      <c r="AN15" s="9"/>
-      <c r="AO15" s="9"/>
-      <c r="AP15" s="9"/>
-      <c r="AQ15" s="9"/>
-      <c r="AR15" s="9"/>
-      <c r="AS15" s="9"/>
-      <c r="AT15" s="9"/>
-      <c r="AU15" s="10"/>
+      <c r="AK15" s="14"/>
+      <c r="AL15" s="15"/>
+      <c r="AM15" s="15"/>
+      <c r="AN15" s="15"/>
+      <c r="AO15" s="15"/>
+      <c r="AP15" s="15"/>
+      <c r="AQ15" s="15"/>
+      <c r="AR15" s="15"/>
+      <c r="AS15" s="15"/>
+      <c r="AT15" s="15"/>
+      <c r="AU15" s="16"/>
     </row>
     <row r="16" spans="2:49" x14ac:dyDescent="0.3">
-      <c r="AK16" s="8"/>
-      <c r="AL16" s="9"/>
-      <c r="AM16" s="9"/>
-      <c r="AN16" s="9"/>
-      <c r="AO16" s="9"/>
-      <c r="AP16" s="9"/>
-      <c r="AQ16" s="9"/>
-      <c r="AR16" s="9"/>
-      <c r="AS16" s="9"/>
-      <c r="AT16" s="9"/>
-      <c r="AU16" s="10"/>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AN16" s="15"/>
+      <c r="AO16" s="15"/>
+      <c r="AP16" s="15"/>
+      <c r="AQ16" s="15"/>
+      <c r="AR16" s="15"/>
+      <c r="AS16" s="15"/>
+      <c r="AT16" s="15"/>
+      <c r="AU16" s="16"/>
     </row>
     <row r="17" spans="37:47" x14ac:dyDescent="0.3">
-      <c r="AK17" s="8"/>
-      <c r="AL17" s="9"/>
-      <c r="AM17" s="9"/>
-      <c r="AN17" s="9"/>
-      <c r="AO17" s="9"/>
-      <c r="AP17" s="9"/>
-      <c r="AQ17" s="9"/>
-      <c r="AR17" s="9"/>
-      <c r="AS17" s="9"/>
-      <c r="AT17" s="9"/>
-      <c r="AU17" s="10"/>
+      <c r="AK17" s="14"/>
+      <c r="AL17" s="15"/>
+      <c r="AM17" s="15"/>
+      <c r="AN17" s="15"/>
+      <c r="AO17" s="15"/>
+      <c r="AP17" s="15"/>
+      <c r="AQ17" s="15"/>
+      <c r="AR17" s="15"/>
+      <c r="AS17" s="15"/>
+      <c r="AT17" s="15"/>
+      <c r="AU17" s="16"/>
     </row>
     <row r="28" spans="37:47" x14ac:dyDescent="0.3">
       <c r="AK28" t="s">
@@ -8418,12 +8398,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B2:AU2"/>
     <mergeCell ref="AK16:AU16"/>
     <mergeCell ref="AK17:AU17"/>
     <mergeCell ref="AK12:AU12"/>
     <mergeCell ref="AK14:AU14"/>
     <mergeCell ref="AK15:AU15"/>
-    <mergeCell ref="B2:AU2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8440,105 +8420,105 @@
   </sheetPr>
   <dimension ref="B1:AL65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AT38" sqref="AT38"/>
+    <sheetView showGridLines="0" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AW29" sqref="AW29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.33203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:38" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:38" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16"/>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
       <c r="AL2" s="2"/>
     </row>
     <row r="3" spans="2:38" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="22"/>
       <c r="AL3" s="4"/>
     </row>
     <row r="4" spans="2:38" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="R11" s="25" t="s">
+      <c r="R11" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="R12" s="22"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="24"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="11"/>
     </row>
     <row r="26" spans="21:21" x14ac:dyDescent="0.3">
       <c r="U26" t="s">
@@ -8576,44 +8556,44 @@
   <sheetData>
     <row r="1" spans="2:38" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:38" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="17"/>
-      <c r="AH2" s="17"/>
-      <c r="AI2" s="17"/>
-      <c r="AJ2" s="17"/>
-      <c r="AK2" s="17"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+      <c r="AG2" s="23"/>
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="23"/>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
       <c r="AL2" s="2"/>
     </row>
     <row r="3" spans="2:38" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8647,44 +8627,44 @@
       <c r="AG3" s="3"/>
     </row>
     <row r="4" spans="2:38" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="12"/>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="12"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
       <c r="AL4" s="4"/>
     </row>
     <row r="5" spans="2:38" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8719,44 +8699,44 @@
   <sheetData>
     <row r="1" spans="2:38" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:38" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="18"/>
-      <c r="AJ2" s="18"/>
-      <c r="AK2" s="18"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
+      <c r="AI2" s="24"/>
+      <c r="AJ2" s="24"/>
+      <c r="AK2" s="24"/>
       <c r="AL2" s="2"/>
     </row>
     <row r="3" spans="2:38" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8790,44 +8770,44 @@
       <c r="AG3" s="3"/>
     </row>
     <row r="4" spans="2:38" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="12"/>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="12"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
       <c r="AL4" s="4"/>
     </row>
     <row r="5" spans="2:38" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8864,44 +8844,44 @@
   <sheetData>
     <row r="1" spans="2:38" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:38" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="25"/>
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
       <c r="AL2" s="2"/>
     </row>
     <row r="3" spans="2:38" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8935,44 +8915,44 @@
       <c r="AG3" s="3"/>
     </row>
     <row r="4" spans="2:38" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="12"/>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="12"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22"/>
       <c r="AL4" s="4"/>
     </row>
     <row r="5" spans="2:38" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9003,6 +8983,131 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <APDescription xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <AssetExpire xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">2029-01-01T08:00:00+00:00</AssetExpire>
+    <CampaignTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </CampaignTagsTaxHTField0>
+    <IntlLangReviewDate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <TPFriendlyName xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <IntlLangReview xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</IntlLangReview>
+    <LocLastLocAttemptVersionLookup xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">848672</LocLastLocAttemptVersionLookup>
+    <PolicheckWords xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <SubmitterId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <AcquiredFrom xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Internal MS</AcquiredFrom>
+    <EditorialStatus xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Complete</EditorialStatus>
+    <Markets xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac"/>
+    <OriginAsset xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <AssetStart xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">2012-07-27T02:51:00+00:00</AssetStart>
+    <FriendlyTitle xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <MarketSpecific xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</MarketSpecific>
+    <TPNamespace xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <PublishStatusLookup xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
+      <Value>455394</Value>
+    </PublishStatusLookup>
+    <APAuthor xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
+      <UserInfo>
+        <DisplayName>REDMOND\v-sa</DisplayName>
+        <AccountId>2467</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </APAuthor>
+    <TPCommandLine xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <IntlLangReviewer xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <OpenTemplate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">true</OpenTemplate>
+    <CSXSubmissionDate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <TaxCatchAll xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac"/>
+    <Manager xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <NumericId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <ParentAssetId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <OriginalSourceMarket xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">english</OriginalSourceMarket>
+    <ApprovalStatus xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">InProgress</ApprovalStatus>
+    <TPComponent xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <EditorialTags xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <TPExecutable xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <TPLaunchHelpLink xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <LocComments xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <LocRecommendedHandoff xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <SourceTitle xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <CSXUpdate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</CSXUpdate>
+    <IntlLocPriority xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <UAProjectedTotalWords xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <AssetType xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">TP</AssetType>
+    <MachineTranslated xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</MachineTranslated>
+    <OutputCachingOn xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</OutputCachingOn>
+    <TemplateStatus xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Complete</TemplateStatus>
+    <IsSearchable xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">true</IsSearchable>
+    <ContentItem xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <HandoffToMSDN xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <ShowIn xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Show everywhere</ShowIn>
+    <ThumbnailAssetId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <UALocComments xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <UALocRecommendation xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Localize</UALocRecommendation>
+    <LastModifiedDateTime xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <LegacyData xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <LocManualTestRequired xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</LocManualTestRequired>
+    <LocMarketGroupTiers2 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <ClipArtFilename xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <TPApplication xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <CSXHash xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <DirectSourceMarket xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">english</DirectSourceMarket>
+    <PrimaryImageGen xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</PrimaryImageGen>
+    <PlannedPubDate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <CSXSubmissionMarket xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <Downloads xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">0</Downloads>
+    <ArtSampleDocs xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <TrustLevel xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">1 Microsoft Managed Content</TrustLevel>
+    <BlockPublish xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</BlockPublish>
+    <TPLaunchHelpLinkType xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Template</TPLaunchHelpLinkType>
+    <LocalizationTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </LocalizationTagsTaxHTField0>
+    <BusinessGroup xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <Providers xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <TemplateTemplateType xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Excel 2007 Default</TemplateTemplateType>
+    <TimesCloned xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <TPAppVersion xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <VoteCount xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <FeatureTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </FeatureTagsTaxHTField0>
+    <Provider xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <UACurrentWords xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <AssetId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">TP103107647</AssetId>
+    <TPClientViewer xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <DSATActionTaken xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <APEditor xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </APEditor>
+    <TPInstallLocation xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <OOCacheId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <IsDeleted xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</IsDeleted>
+    <PublishTargets xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">OfficeOnlineVNext</PublishTargets>
+    <ApprovalLog xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <BugNumber xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <CrawlForDependencies xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</CrawlForDependencies>
+    <InternalTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </InternalTagsTaxHTField0>
+    <LastHandOff xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <Milestone xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <OriginalRelease xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">15</OriginalRelease>
+    <RecommendationsModifier xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+    <ScenarioTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ScenarioTagsTaxHTField0>
+    <UANotes xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x01010062057737089D604C8995D725789FFFFD0400C05BDBFCDB0BE84BA6AEC1D1A4F5E4CE" ma:contentTypeVersion="56" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5c786f17e9890b7d2875e0bb647f603">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dddc4782ba87b44f6678511fd2b89e9" ns2:_="">
     <xsd:import namespace="e5d022ff-4ce9-4922-b5a4-f245e35e2aac"/>
@@ -10036,131 +10141,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <APDescription xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <AssetExpire xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">2029-01-01T08:00:00+00:00</AssetExpire>
-    <CampaignTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </CampaignTagsTaxHTField0>
-    <IntlLangReviewDate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <TPFriendlyName xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <IntlLangReview xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</IntlLangReview>
-    <LocLastLocAttemptVersionLookup xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">848672</LocLastLocAttemptVersionLookup>
-    <PolicheckWords xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <SubmitterId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <AcquiredFrom xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Internal MS</AcquiredFrom>
-    <EditorialStatus xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Complete</EditorialStatus>
-    <Markets xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac"/>
-    <OriginAsset xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <AssetStart xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">2012-07-27T02:51:00+00:00</AssetStart>
-    <FriendlyTitle xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <MarketSpecific xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</MarketSpecific>
-    <TPNamespace xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <PublishStatusLookup xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
-      <Value>455394</Value>
-    </PublishStatusLookup>
-    <APAuthor xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
-      <UserInfo>
-        <DisplayName>REDMOND\v-sa</DisplayName>
-        <AccountId>2467</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </APAuthor>
-    <TPCommandLine xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <IntlLangReviewer xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <OpenTemplate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">true</OpenTemplate>
-    <CSXSubmissionDate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <TaxCatchAll xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac"/>
-    <Manager xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <NumericId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <ParentAssetId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <OriginalSourceMarket xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">english</OriginalSourceMarket>
-    <ApprovalStatus xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">InProgress</ApprovalStatus>
-    <TPComponent xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <EditorialTags xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <TPExecutable xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <TPLaunchHelpLink xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <LocComments xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <LocRecommendedHandoff xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <SourceTitle xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <CSXUpdate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</CSXUpdate>
-    <IntlLocPriority xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <UAProjectedTotalWords xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <AssetType xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">TP</AssetType>
-    <MachineTranslated xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</MachineTranslated>
-    <OutputCachingOn xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</OutputCachingOn>
-    <TemplateStatus xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Complete</TemplateStatus>
-    <IsSearchable xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">true</IsSearchable>
-    <ContentItem xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <HandoffToMSDN xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <ShowIn xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Show everywhere</ShowIn>
-    <ThumbnailAssetId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <UALocComments xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <UALocRecommendation xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Localize</UALocRecommendation>
-    <LastModifiedDateTime xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <LegacyData xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <LocManualTestRequired xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</LocManualTestRequired>
-    <LocMarketGroupTiers2 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <ClipArtFilename xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <TPApplication xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <CSXHash xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <DirectSourceMarket xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">english</DirectSourceMarket>
-    <PrimaryImageGen xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</PrimaryImageGen>
-    <PlannedPubDate xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <CSXSubmissionMarket xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <Downloads xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">0</Downloads>
-    <ArtSampleDocs xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <TrustLevel xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">1 Microsoft Managed Content</TrustLevel>
-    <BlockPublish xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</BlockPublish>
-    <TPLaunchHelpLinkType xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Template</TPLaunchHelpLinkType>
-    <LocalizationTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </LocalizationTagsTaxHTField0>
-    <BusinessGroup xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <Providers xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <TemplateTemplateType xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">Excel 2007 Default</TemplateTemplateType>
-    <TimesCloned xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <TPAppVersion xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <VoteCount xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <FeatureTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </FeatureTagsTaxHTField0>
-    <Provider xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <UACurrentWords xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <AssetId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">TP103107647</AssetId>
-    <TPClientViewer xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <DSATActionTaken xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <APEditor xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </APEditor>
-    <TPInstallLocation xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <OOCacheId xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <IsDeleted xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</IsDeleted>
-    <PublishTargets xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">OfficeOnlineVNext</PublishTargets>
-    <ApprovalLog xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <BugNumber xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <CrawlForDependencies xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">false</CrawlForDependencies>
-    <InternalTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </InternalTagsTaxHTField0>
-    <LastHandOff xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <Milestone xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <OriginalRelease xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">15</OriginalRelease>
-    <RecommendationsModifier xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-    <ScenarioTagsTaxHTField0 xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ScenarioTagsTaxHTField0>
-    <UANotes xmlns="e5d022ff-4ce9-4922-b5a4-f245e35e2aac" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEA305B4-5B15-43B0-97AD-ED100099AAA1}">
   <ds:schemaRefs>
@@ -10170,6 +10150,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D0F3B5-19EE-4272-80BE-E3F25FA5FD34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e5d022ff-4ce9-4922-b5a4-f245e35e2aac"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F89B36D-0441-4E4A-AAB0-33B035B10CD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10185,14 +10175,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D0F3B5-19EE-4272-80BE-E3F25FA5FD34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e5d022ff-4ce9-4922-b5a4-f245e35e2aac"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>